<commit_message>
Repair Libraries location and on recovery...
</commit_message>
<xml_diff>
--- a/Flights GUI E2E UFT Test/Default.xlsx
+++ b/Flights GUI E2E UFT Test/Default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,9 @@
     <sheet name="6 Search Order" sheetId="6" r:id="rId6"/>
     <sheet name="Close Application {External..01" sheetId="7" r:id="rId7"/>
     <sheet name="Close Application {External..02" sheetId="8" r:id="rId8"/>
-    <sheet name="Open Application {External ..00" sheetId="9" r:id="rId9"/>
-    <sheet name="Close Application {External..03" sheetId="10" r:id="rId10"/>
+    <sheet name="Close Application {External..03" sheetId="9" r:id="rId9"/>
+    <sheet name="Open Application {External ..01" sheetId="10" r:id="rId10"/>
+    <sheet name="Close Application {External..00" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -1053,25 +1054,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1379,9 +1380,9 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="10.61328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.61328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.61328125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.01171875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="255" width="9.140625" style="8" customWidth="1"/>
+    <col min="4" max="255" width="9.140625" style="7" customWidth="1"/>
     <col min="256" max="258" width="22.73828125" style="3" bestFit="1" customWidth="1"/>
     <col min="259" max="259" width="9.140625" style="3" customWidth="1"/>
     <col min="260" max="260" width="19.48828125" style="3" bestFit="1" customWidth="1"/>
@@ -2202,13 +2203,13 @@
       </c>
     </row>
     <row r="2" ht="15.1" s="3" customFormat="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>214</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
@@ -2463,7 +2464,7 @@
       <c r="IS2" s="1"/>
       <c r="IT2" s="1"/>
       <c r="IU2" s="1"/>
-      <c r="IV2" s="10"/>
+      <c r="IV2" s="9"/>
       <c r="IW2" s="1"/>
       <c r="IX2" s="1"/>
       <c r="IY2" s="1" t="b">
@@ -2490,18 +2491,18 @@
       <c r="JG2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="JH2" s="7" t="s">
+      <c r="JH2" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" ht="15.1" s="3" customFormat="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -2754,7 +2755,7 @@
       <c r="IS3" s="1"/>
       <c r="IT3" s="1"/>
       <c r="IU3" s="1"/>
-      <c r="IV3" s="10"/>
+      <c r="IV3" s="9"/>
       <c r="IW3" s="1"/>
       <c r="IX3" s="1"/>
       <c r="IY3" s="1"/>
@@ -2766,16 +2767,16 @@
       <c r="JE3" s="1"/>
       <c r="JF3" s="1"/>
       <c r="JG3" s="1"/>
-      <c r="JH3" s="7"/>
+      <c r="JH3" s="8"/>
     </row>
     <row r="4" ht="15.1" s="3" customFormat="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>256</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -3028,7 +3029,7 @@
       <c r="IS4" s="1"/>
       <c r="IT4" s="1"/>
       <c r="IU4" s="1"/>
-      <c r="IV4" s="10"/>
+      <c r="IV4" s="9"/>
       <c r="IW4" s="1"/>
       <c r="IX4" s="1"/>
       <c r="IY4" s="1"/>
@@ -3040,16 +3041,16 @@
       <c r="JE4" s="1"/>
       <c r="JF4" s="1"/>
       <c r="JG4" s="1"/>
-      <c r="JH4" s="7"/>
+      <c r="JH4" s="8"/>
     </row>
     <row r="5" ht="15.1" s="3" customFormat="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>94</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -3302,7 +3303,7 @@
       <c r="IS5" s="1"/>
       <c r="IT5" s="1"/>
       <c r="IU5" s="1"/>
-      <c r="IV5" s="10"/>
+      <c r="IV5" s="9"/>
       <c r="IW5" s="1"/>
       <c r="IX5" s="1"/>
       <c r="IY5" s="1"/>
@@ -3314,12 +3315,12 @@
       <c r="JE5" s="1"/>
       <c r="JF5" s="1"/>
       <c r="JG5" s="1"/>
-      <c r="JH5" s="7"/>
+      <c r="JH5" s="8"/>
     </row>
     <row r="6" ht="15.1">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="4"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -3572,7 +3573,7 @@
       <c r="IS6" s="2"/>
       <c r="IT6" s="2"/>
       <c r="IU6" s="2"/>
-      <c r="IV6" s="10"/>
+      <c r="IV6" s="9"/>
       <c r="IW6" s="1"/>
       <c r="IX6" s="1"/>
       <c r="IY6" s="1"/>
@@ -3584,12 +3585,12 @@
       <c r="JE6" s="1"/>
       <c r="JF6" s="1"/>
       <c r="JG6" s="1"/>
-      <c r="JH6" s="7"/>
+      <c r="JH6" s="8"/>
     </row>
     <row r="7" ht="15.1">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="4"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -3842,7 +3843,7 @@
       <c r="IS7" s="2"/>
       <c r="IT7" s="2"/>
       <c r="IU7" s="2"/>
-      <c r="IV7" s="10"/>
+      <c r="IV7" s="9"/>
       <c r="IW7" s="1"/>
       <c r="IX7" s="1"/>
       <c r="IY7" s="1"/>
@@ -3854,12 +3855,12 @@
       <c r="JE7" s="1"/>
       <c r="JF7" s="1"/>
       <c r="JG7" s="1"/>
-      <c r="JH7" s="7"/>
+      <c r="JH7" s="8"/>
     </row>
     <row r="8" ht="15.1">
-      <c r="A8" s="4"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="4"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -4112,7 +4113,7 @@
       <c r="IS8" s="2"/>
       <c r="IT8" s="2"/>
       <c r="IU8" s="2"/>
-      <c r="IV8" s="10"/>
+      <c r="IV8" s="9"/>
       <c r="IW8" s="1"/>
       <c r="IX8" s="1"/>
       <c r="IY8" s="1"/>
@@ -4124,12 +4125,12 @@
       <c r="JE8" s="1"/>
       <c r="JF8" s="1"/>
       <c r="JG8" s="1"/>
-      <c r="JH8" s="7"/>
+      <c r="JH8" s="8"/>
     </row>
     <row r="9" ht="15.1">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="4"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -4382,7 +4383,7 @@
       <c r="IS9" s="2"/>
       <c r="IT9" s="2"/>
       <c r="IU9" s="2"/>
-      <c r="IV9" s="10"/>
+      <c r="IV9" s="9"/>
       <c r="IW9" s="1"/>
       <c r="IX9" s="1"/>
       <c r="IY9" s="1"/>
@@ -4394,12 +4395,12 @@
       <c r="JE9" s="1"/>
       <c r="JF9" s="1"/>
       <c r="JG9" s="1"/>
-      <c r="JH9" s="7"/>
+      <c r="JH9" s="8"/>
     </row>
     <row r="10" ht="15.1">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -4652,7 +4653,7 @@
       <c r="IS10" s="2"/>
       <c r="IT10" s="2"/>
       <c r="IU10" s="2"/>
-      <c r="IV10" s="10"/>
+      <c r="IV10" s="9"/>
       <c r="IW10" s="1"/>
       <c r="IX10" s="1"/>
       <c r="IY10" s="1"/>
@@ -4664,12 +4665,12 @@
       <c r="JE10" s="1"/>
       <c r="JF10" s="1"/>
       <c r="JG10" s="1"/>
-      <c r="JH10" s="7"/>
+      <c r="JH10" s="8"/>
     </row>
     <row r="11" ht="15.1">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="4"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -4922,7 +4923,7 @@
       <c r="IS11" s="2"/>
       <c r="IT11" s="2"/>
       <c r="IU11" s="2"/>
-      <c r="IV11" s="10"/>
+      <c r="IV11" s="9"/>
       <c r="IW11" s="1"/>
       <c r="IX11" s="1"/>
       <c r="IY11" s="1"/>
@@ -4934,7 +4935,7 @@
       <c r="JE11" s="1"/>
       <c r="JF11" s="1"/>
       <c r="JG11" s="1"/>
-      <c r="JH11" s="7"/>
+      <c r="JH11" s="8"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -4951,13 +4952,32 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.95"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="5" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customFormat="1"/>
@@ -5071,9 +5091,9 @@
       </c>
     </row>
     <row r="2" s="3" customFormat="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="7" t="b">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5114,7 +5134,7 @@
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="9" t="str">
+      <c r="B2" s="10" t="str">
         <f t="shared" si="0" ref="B2:B8">"DSN=Flight;Database=C:\Users\"&amp;A2&amp;"\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD="</f>
         <v>DSN=Flight;Database=C:\Users\someone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -5123,7 +5143,7 @@
       <c r="A3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="9" t="str">
+      <c r="B3" s="10" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flight;Database=C:\Users\someone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -5132,7 +5152,7 @@
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="9" t="str">
+      <c r="B4" s="10" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flight;Database=C:\Users\someone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -5141,7 +5161,7 @@
       <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="9" t="str">
+      <c r="B5" s="10" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flight;Database=C:\Users\someone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -5150,7 +5170,7 @@
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="9" t="str">
+      <c r="B6" s="10" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flight;Database=C:\Users\someone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -5159,7 +5179,7 @@
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="9" t="str">
+      <c r="B7" s="10" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flight;Database=C:\Users\someone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -5168,7 +5188,7 @@
       <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="9" t="str">
+      <c r="B8" s="10" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flight;Database=C:\Users\someone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -5193,7 +5213,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="5" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customFormat="1"/>
@@ -5212,7 +5232,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="5" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customFormat="1"/>
@@ -5231,7 +5251,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="5" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customFormat="1"/>

</xml_diff>